<commit_message>
Added Sbase and Vbase
Sbase values are in single phase now
Vbase values are sent as individual value
</commit_message>
<xml_diff>
--- a/Documentations/Datasets/IEEE 33 CDF (Updated).xlsx
+++ b/Documentations/Datasets/IEEE 33 CDF (Updated).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\Ladder-Iterative-Loadflow\Documentations\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E4993D-5D23-4810-B1C4-6BAD6B75386F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F3041B-16F7-464F-BDE9-72194363B708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{AE3323F2-0094-4B0C-9BAF-50E26493BB40}"/>
+    <workbookView xWindow="-24960" yWindow="1080" windowWidth="21600" windowHeight="11475" xr2:uid="{AE3323F2-0094-4B0C-9BAF-50E26493BB40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="66">
   <si>
     <t>END OF DATA</t>
   </si>
@@ -220,6 +220,18 @@
   </si>
   <si>
     <t>Maximum Power</t>
+  </si>
+  <si>
+    <t>Power is MegaWat</t>
+  </si>
+  <si>
+    <t>Vb is kV</t>
+  </si>
+  <si>
+    <t>&lt;- This is 3phase</t>
+  </si>
+  <si>
+    <t>This is line to line</t>
   </si>
 </sst>
 </file>
@@ -629,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02368925-FB68-47DE-A660-EAA97F9F58F2}">
-  <dimension ref="A1:U85"/>
+  <dimension ref="A1:X85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -643,12 +655,12 @@
     <col min="8" max="20" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:24">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:24">
       <c r="A2" s="4"/>
       <c r="F2" s="14" t="s">
         <v>56</v>
@@ -659,7 +671,7 @@
       </c>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:24">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -682,7 +694,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:24">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -738,7 +750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:24">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -793,8 +805,14 @@
       <c r="R5" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:18">
+      <c r="V5" t="s">
+        <v>62</v>
+      </c>
+      <c r="X5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -849,8 +867,14 @@
       <c r="R6" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:18">
+      <c r="V6" t="s">
+        <v>63</v>
+      </c>
+      <c r="X6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -906,7 +930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:24">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -962,7 +986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:24">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -1018,7 +1042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:24">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -1074,7 +1098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:24">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -1130,7 +1154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:24">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -1186,7 +1210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:24">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -1242,7 +1266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:24">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -1298,7 +1322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:24">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -1354,7 +1378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:24">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -5075,15 +5099,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010025B10B9F6FFF7142B7B32A4A4A47FA43" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="66c3d941594396c273f2733aaa9e4491">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="034b7289-f67f-4149-bf72-e8ff36efdb2e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6a3e312227fdd923874c5297960ecd80" ns3:_="">
     <xsd:import namespace="034b7289-f67f-4149-bf72-e8ff36efdb2e"/>
@@ -5215,6 +5230,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -5222,14 +5246,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0524FC3A-FFBB-4947-8673-B2AD9D6D8986}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE4B6B2C-9891-4227-91D2-DF310237F6D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5243,6 +5259,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0524FC3A-FFBB-4947-8673-B2AD9D6D8986}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>